<commit_message>
Quite a few fixes :P Make sure you say "End" at the end, not "end".
</commit_message>
<xml_diff>
--- a/Assets/Songs/Music Translator workbook.xlsx
+++ b/Assets/Songs/Music Translator workbook.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpwelsh\Desktop\Beatrider\Assets\Songs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielsSickPC\Desktop\BeatRider\Assets\Songs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27160" windowHeight="13130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27165" windowHeight="13125"/>
   </bookViews>
   <sheets>
     <sheet name="Music Translator" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>A</t>
   </si>
@@ -82,12 +82,15 @@
   </si>
   <si>
     <t>what we use</t>
+  </si>
+  <si>
+    <t>End</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -594,16 +597,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -744,6 +747,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -779,6 +799,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -934,43 +971,43 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D17" t="s">
@@ -1001,7 +1038,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1033,18 +1070,18 @@
         <v>17</v>
       </c>
       <c r="K18" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B22" s="5" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D22" t="s">
@@ -1075,52 +1112,52 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="6" t="str">
-        <f>IF(EXACT(B22,"g"),"A",IF(EXACT(B22,"a"),"S",IF(B22="B","D",IF(B22="C","F",IF(B22="D","G",IF(B22="E","H",IF(B22="F","J",IF(B22="G","K",IF(B22="A","L",IF(B22="end","end",""))))))))))</f>
+      <c r="B23" s="4" t="str">
+        <f t="shared" ref="B23:L23" si="0">IF(EXACT(B22,"g"),"A",IF(EXACT(B22,"a"),"S",IF(B22="B","D",IF(B22="C","F",IF(B22="D","G",IF(B22="E","H",IF(B22="F","J",IF(B22="G","K",IF(B22="A","L",IF(B22="end","end",""))))))))))</f>
         <v>A</v>
       </c>
-      <c r="C23" s="6" t="str">
-        <f>IF(EXACT(C22,"g"),"A",IF(EXACT(C22,"a"),"S",IF(C22="B","D",IF(C22="C","F",IF(C22="D","G",IF(C22="E","H",IF(C22="F","J",IF(C22="G","K",IF(C22="A","L",IF(C22="end","end",""))))))))))</f>
+      <c r="C23" s="4" t="str">
+        <f t="shared" si="0"/>
         <v>S</v>
       </c>
-      <c r="D23" s="6" t="str">
-        <f>IF(EXACT(D22,"g"),"A",IF(EXACT(D22,"a"),"S",IF(D22="B","D",IF(D22="C","F",IF(D22="D","G",IF(D22="E","H",IF(D22="F","J",IF(D22="G","K",IF(D22="A","L",IF(D22="end","end",""))))))))))</f>
+      <c r="D23" s="4" t="str">
+        <f t="shared" si="0"/>
         <v>D</v>
       </c>
-      <c r="E23" s="6" t="str">
-        <f>IF(EXACT(E22,"g"),"A",IF(EXACT(E22,"a"),"S",IF(E22="B","D",IF(E22="C","F",IF(E22="D","G",IF(E22="E","H",IF(E22="F","J",IF(E22="G","K",IF(E22="A","L",IF(E22="end","end",""))))))))))</f>
+      <c r="E23" s="4" t="str">
+        <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="F23" s="6" t="str">
-        <f>IF(EXACT(F22,"g"),"A",IF(EXACT(F22,"a"),"S",IF(F22="B","D",IF(F22="C","F",IF(F22="D","G",IF(F22="E","H",IF(F22="F","J",IF(F22="G","K",IF(F22="A","L",IF(F22="end","end",""))))))))))</f>
+      <c r="F23" s="4" t="str">
+        <f t="shared" si="0"/>
         <v>G</v>
       </c>
-      <c r="G23" s="6" t="str">
-        <f>IF(EXACT(G22,"g"),"A",IF(EXACT(G22,"a"),"S",IF(G22="B","D",IF(G22="C","F",IF(G22="D","G",IF(G22="E","H",IF(G22="F","J",IF(G22="G","K",IF(G22="A","L",IF(G22="end","end",""))))))))))</f>
+      <c r="G23" s="4" t="str">
+        <f t="shared" si="0"/>
         <v>H</v>
       </c>
-      <c r="H23" s="6" t="str">
-        <f>IF(EXACT(H22,"g"),"A",IF(EXACT(H22,"a"),"S",IF(H22="B","D",IF(H22="C","F",IF(H22="D","G",IF(H22="E","H",IF(H22="F","J",IF(H22="G","K",IF(H22="A","L",IF(H22="end","end",""))))))))))</f>
+      <c r="H23" s="4" t="str">
+        <f t="shared" si="0"/>
         <v>J</v>
       </c>
-      <c r="I23" s="6" t="str">
-        <f>IF(EXACT(I22,"g"),"A",IF(EXACT(I22,"a"),"S",IF(I22="B","D",IF(I22="C","F",IF(I22="D","G",IF(I22="E","H",IF(I22="F","J",IF(I22="G","K",IF(I22="A","L",IF(I22="end","end",""))))))))))</f>
+      <c r="I23" s="4" t="str">
+        <f t="shared" si="0"/>
         <v>K</v>
       </c>
-      <c r="J23" s="6" t="str">
-        <f>IF(EXACT(J22,"g"),"A",IF(EXACT(J22,"a"),"S",IF(J22="B","D",IF(J22="C","F",IF(J22="D","G",IF(J22="E","H",IF(J22="F","J",IF(J22="G","K",IF(J22="A","L",IF(J22="end","end",""))))))))))</f>
+      <c r="J23" s="4" t="str">
+        <f t="shared" si="0"/>
         <v>L</v>
       </c>
-      <c r="K23" s="6" t="str">
-        <f>IF(EXACT(K22,"g"),"A",IF(EXACT(K22,"a"),"S",IF(K22="B","D",IF(K22="C","F",IF(K22="D","G",IF(K22="E","H",IF(K22="F","J",IF(K22="G","K",IF(K22="A","L",IF(K22="end","end",""))))))))))</f>
-        <v>end</v>
+      <c r="K23" s="4" t="str">
+        <f>IF(EXACT(K22,"g"),"A",IF(EXACT(K22,"a"),"S",IF(K22="B","D",IF(K22="C","F",IF(K22="D","G",IF(K22="E","H",IF(K22="F","J",IF(K22="G","K",IF(K22="A","L",IF(K22="end","End",""))))))))))</f>
+        <v>End</v>
       </c>
       <c r="L23" t="str">
-        <f>IF(EXACT(L22,"g"),"A",IF(EXACT(L22,"a"),"S",IF(L22="B","D",IF(L22="C","F",IF(L22="D","G",IF(L22="E","H",IF(L22="F","J",IF(L22="G","K",IF(L22="A","L",IF(L22="end","end",""))))))))))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>

</xml_diff>